<commit_message>
excel import to Store model(+ add fields)
</commit_message>
<xml_diff>
--- a/crawling/data/yogiyo_홍익대_final.xlsx
+++ b/crawling/data/yogiyo_홍익대_final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\error_fix\crawling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7330131-8843-4B19-9319-EC8DB8EDC6B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058F330E-032A-49AB-B533-24E35E57411D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="치킨" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6831" uniqueCount="2612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6978" uniqueCount="2612">
   <si>
     <t>상세페이지URL</t>
   </si>
@@ -8263,7 +8263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -12225,12 +12225,13 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="24.875" customWidth="1"/>
+    <col min="5" max="5" width="37.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -12473,8 +12474,14 @@
       <c r="C11" t="s">
         <v>750</v>
       </c>
+      <c r="D11" t="s">
+        <v>2602</v>
+      </c>
       <c r="E11" t="s">
         <v>56</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2602</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -12490,6 +12497,9 @@
       <c r="C12" t="s">
         <v>752</v>
       </c>
+      <c r="D12" t="s">
+        <v>2602</v>
+      </c>
       <c r="E12" t="s">
         <v>56</v>
       </c>
@@ -12510,8 +12520,14 @@
       <c r="C13" t="s">
         <v>754</v>
       </c>
+      <c r="D13" t="s">
+        <v>2602</v>
+      </c>
       <c r="E13" t="s">
         <v>56</v>
+      </c>
+      <c r="F13" t="s">
+        <v>2602</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -12527,8 +12543,14 @@
       <c r="C14" t="s">
         <v>756</v>
       </c>
+      <c r="D14" t="s">
+        <v>2602</v>
+      </c>
       <c r="E14" t="s">
         <v>56</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2602</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -12544,8 +12566,14 @@
       <c r="C15" t="s">
         <v>758</v>
       </c>
+      <c r="D15" t="s">
+        <v>2602</v>
+      </c>
       <c r="E15" t="s">
         <v>56</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2602</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -12561,8 +12589,14 @@
       <c r="C16" t="s">
         <v>760</v>
       </c>
+      <c r="D16" t="s">
+        <v>2602</v>
+      </c>
       <c r="E16" t="s">
         <v>56</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2602</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
@@ -12578,8 +12612,14 @@
       <c r="C17" t="s">
         <v>762</v>
       </c>
+      <c r="D17" t="s">
+        <v>2602</v>
+      </c>
       <c r="E17" t="s">
         <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2602</v>
       </c>
       <c r="G17" s="1">
         <v>0</v>
@@ -12595,8 +12635,14 @@
       <c r="C18" t="s">
         <v>764</v>
       </c>
+      <c r="D18" t="s">
+        <v>2602</v>
+      </c>
       <c r="E18" t="s">
         <v>56</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2602</v>
       </c>
       <c r="G18" s="1">
         <v>0</v>
@@ -12612,8 +12658,14 @@
       <c r="C19" t="s">
         <v>766</v>
       </c>
+      <c r="D19" t="s">
+        <v>2602</v>
+      </c>
       <c r="E19" t="s">
         <v>56</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2602</v>
       </c>
       <c r="G19" s="1">
         <v>0</v>
@@ -16564,11 +16616,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B6D53D-C65F-4CE8-951B-47D35AB80854}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I78" sqref="I78"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="48.75" customWidth="1"/>
+    <col min="2" max="2" width="34.5" customWidth="1"/>
+    <col min="3" max="3" width="34.625" customWidth="1"/>
+    <col min="4" max="4" width="24.125" customWidth="1"/>
+    <col min="5" max="5" width="25.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -17391,6 +17450,9 @@
       <c r="E36" t="s">
         <v>31</v>
       </c>
+      <c r="F36" t="s">
+        <v>2602</v>
+      </c>
       <c r="G36" s="1">
         <v>21</v>
       </c>
@@ -18003,8 +18065,14 @@
       <c r="C63" t="s">
         <v>2104</v>
       </c>
+      <c r="D63" t="s">
+        <v>2602</v>
+      </c>
       <c r="E63" t="s">
         <v>45</v>
+      </c>
+      <c r="F63" t="s">
+        <v>2602</v>
       </c>
       <c r="G63" s="1">
         <v>0</v>
@@ -18020,8 +18088,14 @@
       <c r="C64" t="s">
         <v>2107</v>
       </c>
+      <c r="D64" t="s">
+        <v>2602</v>
+      </c>
       <c r="E64" t="s">
         <v>17</v>
+      </c>
+      <c r="F64" t="s">
+        <v>2602</v>
       </c>
       <c r="G64" s="1">
         <v>0</v>
@@ -18037,8 +18111,14 @@
       <c r="C65" t="s">
         <v>2110</v>
       </c>
+      <c r="D65" t="s">
+        <v>2602</v>
+      </c>
       <c r="E65" t="s">
         <v>17</v>
+      </c>
+      <c r="F65" t="s">
+        <v>2602</v>
       </c>
       <c r="G65" s="1">
         <v>0</v>
@@ -18054,8 +18134,14 @@
       <c r="C66" t="s">
         <v>2113</v>
       </c>
+      <c r="D66" t="s">
+        <v>2602</v>
+      </c>
       <c r="E66" t="s">
         <v>17</v>
+      </c>
+      <c r="F66" t="s">
+        <v>2602</v>
       </c>
       <c r="G66" s="1">
         <v>0</v>
@@ -18071,6 +18157,9 @@
       <c r="C67" t="s">
         <v>2116</v>
       </c>
+      <c r="D67" t="s">
+        <v>2602</v>
+      </c>
       <c r="E67" t="s">
         <v>17</v>
       </c>
@@ -18091,8 +18180,14 @@
       <c r="C68" t="s">
         <v>2119</v>
       </c>
+      <c r="D68" t="s">
+        <v>2602</v>
+      </c>
       <c r="E68" t="s">
         <v>252</v>
+      </c>
+      <c r="F68" t="s">
+        <v>2602</v>
       </c>
       <c r="G68" s="1">
         <v>0</v>
@@ -18108,8 +18203,14 @@
       <c r="C69" t="s">
         <v>2122</v>
       </c>
+      <c r="D69" t="s">
+        <v>2602</v>
+      </c>
       <c r="E69" t="s">
         <v>252</v>
+      </c>
+      <c r="F69" t="s">
+        <v>2602</v>
       </c>
       <c r="G69" s="1">
         <v>0</v>
@@ -18125,6 +18226,9 @@
       <c r="C70" t="s">
         <v>2125</v>
       </c>
+      <c r="D70" t="s">
+        <v>2602</v>
+      </c>
       <c r="E70" t="s">
         <v>72</v>
       </c>
@@ -18145,8 +18249,14 @@
       <c r="C71" t="s">
         <v>2128</v>
       </c>
+      <c r="D71" t="s">
+        <v>2602</v>
+      </c>
       <c r="E71" t="s">
         <v>17</v>
+      </c>
+      <c r="F71" t="s">
+        <v>2602</v>
       </c>
       <c r="G71" s="1">
         <v>0</v>
@@ -18162,8 +18272,14 @@
       <c r="C72" t="s">
         <v>2131</v>
       </c>
+      <c r="D72" t="s">
+        <v>2602</v>
+      </c>
       <c r="E72" t="s">
         <v>56</v>
+      </c>
+      <c r="F72" t="s">
+        <v>2602</v>
       </c>
       <c r="G72" s="1">
         <v>0</v>
@@ -18179,8 +18295,14 @@
       <c r="C73" t="s">
         <v>2134</v>
       </c>
+      <c r="D73" t="s">
+        <v>2602</v>
+      </c>
       <c r="E73" t="s">
         <v>39</v>
+      </c>
+      <c r="F73" t="s">
+        <v>2602</v>
       </c>
       <c r="G73" s="1">
         <v>0</v>
@@ -18196,8 +18318,14 @@
       <c r="C74" t="s">
         <v>2136</v>
       </c>
+      <c r="D74" t="s">
+        <v>2602</v>
+      </c>
       <c r="E74" t="s">
         <v>39</v>
+      </c>
+      <c r="F74" t="s">
+        <v>2602</v>
       </c>
       <c r="G74" s="1">
         <v>0</v>
@@ -18213,8 +18341,14 @@
       <c r="C75" t="s">
         <v>2138</v>
       </c>
+      <c r="D75" t="s">
+        <v>2602</v>
+      </c>
       <c r="E75" t="s">
         <v>39</v>
+      </c>
+      <c r="F75" t="s">
+        <v>2602</v>
       </c>
       <c r="G75" s="1">
         <v>0</v>
@@ -18230,8 +18364,14 @@
       <c r="C76" t="s">
         <v>2140</v>
       </c>
+      <c r="D76" t="s">
+        <v>2602</v>
+      </c>
       <c r="E76" t="s">
         <v>39</v>
+      </c>
+      <c r="F76" t="s">
+        <v>2602</v>
       </c>
       <c r="G76" s="1">
         <v>0</v>
@@ -18247,8 +18387,14 @@
       <c r="C77" t="s">
         <v>2142</v>
       </c>
+      <c r="D77" t="s">
+        <v>2602</v>
+      </c>
       <c r="E77" t="s">
         <v>39</v>
+      </c>
+      <c r="F77" t="s">
+        <v>2602</v>
       </c>
       <c r="G77" s="1">
         <v>0</v>
@@ -18264,8 +18410,14 @@
       <c r="C78" t="s">
         <v>2145</v>
       </c>
+      <c r="D78" t="s">
+        <v>2602</v>
+      </c>
       <c r="E78" t="s">
         <v>2146</v>
+      </c>
+      <c r="F78" t="s">
+        <v>2602</v>
       </c>
       <c r="G78" s="1">
         <v>0</v>
@@ -18281,8 +18433,14 @@
       <c r="C79" t="s">
         <v>2149</v>
       </c>
+      <c r="D79" t="s">
+        <v>2602</v>
+      </c>
       <c r="E79" t="s">
         <v>1140</v>
+      </c>
+      <c r="F79" t="s">
+        <v>2602</v>
       </c>
       <c r="G79" s="1">
         <v>0</v>
@@ -18298,8 +18456,14 @@
       <c r="C80" t="s">
         <v>2191</v>
       </c>
+      <c r="D80" t="s">
+        <v>2602</v>
+      </c>
       <c r="E80" t="s">
         <v>31</v>
+      </c>
+      <c r="F80" t="s">
+        <v>2602</v>
       </c>
       <c r="G80" s="1">
         <v>0</v>
@@ -18315,8 +18479,14 @@
       <c r="C81" t="s">
         <v>2193</v>
       </c>
+      <c r="D81" t="s">
+        <v>2602</v>
+      </c>
       <c r="E81" t="s">
         <v>31</v>
+      </c>
+      <c r="F81" t="s">
+        <v>2602</v>
       </c>
       <c r="G81" s="1">
         <v>0</v>
@@ -18332,8 +18502,14 @@
       <c r="C82" t="s">
         <v>2196</v>
       </c>
+      <c r="D82" t="s">
+        <v>2602</v>
+      </c>
       <c r="E82" t="s">
         <v>31</v>
+      </c>
+      <c r="F82" t="s">
+        <v>2602</v>
       </c>
       <c r="G82" s="1">
         <v>0</v>
@@ -18345,6 +18521,7 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18352,14 +18529,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AABF1E81-7C67-467D-BD2A-D1AC5991E380}">
   <dimension ref="A1:G239"/>
   <sheetViews>
-    <sheetView topLeftCell="C214" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="99.625" customWidth="1"/>
     <col min="3" max="3" width="45.625" customWidth="1"/>
+    <col min="5" max="5" width="26.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -18539,6 +18717,9 @@
       <c r="E8" t="s">
         <v>39</v>
       </c>
+      <c r="F8" t="s">
+        <v>2602</v>
+      </c>
       <c r="G8" s="1">
         <v>1533</v>
       </c>
@@ -20238,6 +20419,9 @@
       <c r="E82" t="s">
         <v>17</v>
       </c>
+      <c r="F82" t="s">
+        <v>2602</v>
+      </c>
       <c r="G82" s="1">
         <v>128</v>
       </c>
@@ -20672,6 +20856,9 @@
       <c r="E101" t="s">
         <v>303</v>
       </c>
+      <c r="F101" t="s">
+        <v>2602</v>
+      </c>
       <c r="G101" s="1">
         <v>80</v>
       </c>
@@ -20968,6 +21155,9 @@
       <c r="E114" t="s">
         <v>31</v>
       </c>
+      <c r="F114" t="s">
+        <v>2602</v>
+      </c>
       <c r="G114" s="1">
         <v>60</v>
       </c>
@@ -22391,6 +22581,9 @@
       <c r="E176" t="s">
         <v>31</v>
       </c>
+      <c r="F176" t="s">
+        <v>2602</v>
+      </c>
       <c r="G176" s="1">
         <v>11</v>
       </c>
@@ -23515,6 +23708,9 @@
       <c r="E225" t="s">
         <v>289</v>
       </c>
+      <c r="F225" t="s">
+        <v>2602</v>
+      </c>
       <c r="G225" s="1">
         <v>2</v>
       </c>
@@ -23650,6 +23846,9 @@
       <c r="E231" t="s">
         <v>11</v>
       </c>
+      <c r="F231" t="s">
+        <v>2602</v>
+      </c>
       <c r="G231" s="1">
         <v>2</v>
       </c>
@@ -23762,6 +23961,9 @@
       <c r="E236" t="s">
         <v>39</v>
       </c>
+      <c r="F236" t="s">
+        <v>2602</v>
+      </c>
       <c r="G236" s="1">
         <v>1</v>
       </c>
@@ -23804,6 +24006,9 @@
       </c>
       <c r="E238" t="s">
         <v>403</v>
+      </c>
+      <c r="F238" t="s">
+        <v>2602</v>
       </c>
       <c r="G238" s="1">
         <v>1</v>
@@ -23846,11 +24051,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C0B9671-12B0-4375-B259-9F5F2FC5E9AE}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="I97" sqref="I97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="39.25" customWidth="1"/>
+    <col min="5" max="5" width="25.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -24719,6 +24928,9 @@
       <c r="E38" t="s">
         <v>680</v>
       </c>
+      <c r="F38" t="s">
+        <v>2602</v>
+      </c>
       <c r="G38" s="1">
         <v>90</v>
       </c>
@@ -25222,6 +25434,9 @@
       <c r="E60" t="s">
         <v>252</v>
       </c>
+      <c r="F60" t="s">
+        <v>2602</v>
+      </c>
       <c r="G60" s="1">
         <v>26</v>
       </c>
@@ -25288,6 +25503,9 @@
       <c r="E63" t="s">
         <v>241</v>
       </c>
+      <c r="F63" t="s">
+        <v>2602</v>
+      </c>
       <c r="G63">
         <v>23</v>
       </c>
@@ -25768,6 +25986,9 @@
       <c r="E84" t="s">
         <v>99</v>
       </c>
+      <c r="F84" t="s">
+        <v>2602</v>
+      </c>
       <c r="G84" s="1">
         <v>2</v>
       </c>
@@ -25834,6 +26055,9 @@
       <c r="E87" t="s">
         <v>31</v>
       </c>
+      <c r="F87" t="s">
+        <v>2602</v>
+      </c>
       <c r="G87" s="1">
         <v>1</v>
       </c>
@@ -25900,6 +26124,9 @@
       <c r="E90" t="s">
         <v>39</v>
       </c>
+      <c r="F90" t="s">
+        <v>2602</v>
+      </c>
       <c r="G90" s="1">
         <v>1</v>
       </c>
@@ -25914,8 +26141,14 @@
       <c r="C91" t="s">
         <v>577</v>
       </c>
+      <c r="D91" t="s">
+        <v>2602</v>
+      </c>
       <c r="E91" t="s">
         <v>160</v>
+      </c>
+      <c r="F91" t="s">
+        <v>2602</v>
       </c>
       <c r="G91" s="1">
         <v>0</v>
@@ -25931,6 +26164,9 @@
       <c r="C92" t="s">
         <v>580</v>
       </c>
+      <c r="D92" t="s">
+        <v>2602</v>
+      </c>
       <c r="E92" t="s">
         <v>99</v>
       </c>
@@ -25951,6 +26187,9 @@
       <c r="C93" t="s">
         <v>583</v>
       </c>
+      <c r="D93" t="s">
+        <v>2602</v>
+      </c>
       <c r="E93" t="s">
         <v>39</v>
       </c>
@@ -25971,8 +26210,14 @@
       <c r="C94" t="s">
         <v>587</v>
       </c>
+      <c r="D94" t="s">
+        <v>2602</v>
+      </c>
       <c r="E94" t="s">
         <v>39</v>
+      </c>
+      <c r="F94" t="s">
+        <v>2602</v>
       </c>
       <c r="G94" s="1">
         <v>0</v>
@@ -25988,8 +26233,14 @@
       <c r="C95" t="s">
         <v>590</v>
       </c>
+      <c r="D95" t="s">
+        <v>2602</v>
+      </c>
       <c r="E95" t="s">
         <v>56</v>
+      </c>
+      <c r="F95" t="s">
+        <v>2602</v>
       </c>
       <c r="G95" s="1">
         <v>0</v>
@@ -26005,8 +26256,14 @@
       <c r="C96" t="s">
         <v>593</v>
       </c>
+      <c r="D96" t="s">
+        <v>2602</v>
+      </c>
       <c r="E96" t="s">
         <v>31</v>
+      </c>
+      <c r="F96" t="s">
+        <v>2602</v>
       </c>
       <c r="G96" s="1">
         <v>0</v>
@@ -26022,8 +26279,14 @@
       <c r="C97" t="s">
         <v>596</v>
       </c>
+      <c r="D97" t="s">
+        <v>2602</v>
+      </c>
       <c r="E97" t="s">
         <v>45</v>
+      </c>
+      <c r="F97" t="s">
+        <v>2602</v>
       </c>
       <c r="G97" s="1">
         <v>0</v>
@@ -26039,8 +26302,14 @@
       <c r="C98" t="s">
         <v>598</v>
       </c>
+      <c r="D98" t="s">
+        <v>2602</v>
+      </c>
       <c r="E98" t="s">
         <v>45</v>
+      </c>
+      <c r="F98" t="s">
+        <v>2602</v>
       </c>
       <c r="G98" s="1">
         <v>0</v>
@@ -26056,8 +26325,14 @@
       <c r="C99" t="s">
         <v>601</v>
       </c>
+      <c r="D99" t="s">
+        <v>2602</v>
+      </c>
       <c r="E99" t="s">
         <v>289</v>
+      </c>
+      <c r="F99" t="s">
+        <v>2602</v>
       </c>
       <c r="G99" s="1">
         <v>0</v>
@@ -26073,8 +26348,14 @@
       <c r="C100" t="s">
         <v>604</v>
       </c>
+      <c r="D100" t="s">
+        <v>2602</v>
+      </c>
       <c r="E100" t="s">
         <v>241</v>
+      </c>
+      <c r="F100" t="s">
+        <v>2602</v>
       </c>
       <c r="G100" s="1">
         <v>0</v>
@@ -26090,8 +26371,14 @@
       <c r="C101" t="s">
         <v>607</v>
       </c>
+      <c r="D101" t="s">
+        <v>2602</v>
+      </c>
       <c r="E101" t="s">
         <v>241</v>
+      </c>
+      <c r="F101" t="s">
+        <v>2602</v>
       </c>
       <c r="G101" s="1">
         <v>0</v>
@@ -26107,8 +26394,14 @@
       <c r="C102" t="s">
         <v>610</v>
       </c>
+      <c r="D102" t="s">
+        <v>2602</v>
+      </c>
       <c r="E102" t="s">
         <v>241</v>
+      </c>
+      <c r="F102" t="s">
+        <v>2602</v>
       </c>
       <c r="G102" s="1">
         <v>0</v>
@@ -26127,13 +26420,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDFF813B-216F-4E99-B606-B6FEBAEA7E34}">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H70" sqref="H70"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="38.75" customWidth="1"/>
+    <col min="4" max="4" width="29.125" customWidth="1"/>
+    <col min="5" max="5" width="29.875" customWidth="1"/>
     <col min="6" max="6" width="35.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -26797,6 +27092,9 @@
       <c r="E29" t="s">
         <v>17</v>
       </c>
+      <c r="F29" t="s">
+        <v>2602</v>
+      </c>
       <c r="G29" s="1">
         <v>128</v>
       </c>
@@ -26817,6 +27115,9 @@
       <c r="E30" t="s">
         <v>241</v>
       </c>
+      <c r="F30" t="s">
+        <v>2602</v>
+      </c>
       <c r="G30" s="1">
         <v>118</v>
       </c>
@@ -26860,6 +27161,9 @@
       <c r="E32" t="s">
         <v>31</v>
       </c>
+      <c r="F32" t="s">
+        <v>2602</v>
+      </c>
       <c r="G32" s="1">
         <v>102</v>
       </c>
@@ -27110,6 +27414,9 @@
       <c r="E43" t="s">
         <v>289</v>
       </c>
+      <c r="F43" t="s">
+        <v>2602</v>
+      </c>
       <c r="G43" s="1">
         <v>40</v>
       </c>
@@ -27314,6 +27621,9 @@
       <c r="E52" t="s">
         <v>403</v>
       </c>
+      <c r="F52" t="s">
+        <v>2602</v>
+      </c>
       <c r="G52" s="1">
         <v>5</v>
       </c>
@@ -27403,6 +27713,9 @@
       <c r="E56" t="s">
         <v>410</v>
       </c>
+      <c r="F56" t="s">
+        <v>2602</v>
+      </c>
       <c r="G56" s="1">
         <v>1</v>
       </c>
@@ -27423,6 +27736,9 @@
       <c r="E57" t="s">
         <v>241</v>
       </c>
+      <c r="F57" t="s">
+        <v>2602</v>
+      </c>
       <c r="G57" s="1">
         <v>1</v>
       </c>
@@ -27466,6 +27782,9 @@
       <c r="E59" t="s">
         <v>252</v>
       </c>
+      <c r="F59" t="s">
+        <v>2602</v>
+      </c>
       <c r="G59" s="1">
         <v>1</v>
       </c>
@@ -27486,6 +27805,9 @@
       <c r="E60" t="s">
         <v>289</v>
       </c>
+      <c r="F60" t="s">
+        <v>2602</v>
+      </c>
       <c r="G60" s="1">
         <v>1</v>
       </c>
@@ -27500,8 +27822,14 @@
       <c r="C61" t="s">
         <v>425</v>
       </c>
+      <c r="D61" t="s">
+        <v>2602</v>
+      </c>
       <c r="E61" t="s">
         <v>17</v>
+      </c>
+      <c r="F61" t="s">
+        <v>2602</v>
       </c>
       <c r="G61" s="1">
         <v>0</v>
@@ -27517,6 +27845,9 @@
       <c r="C62" t="s">
         <v>428</v>
       </c>
+      <c r="D62" t="s">
+        <v>2602</v>
+      </c>
       <c r="E62" t="s">
         <v>56</v>
       </c>
@@ -27537,8 +27868,14 @@
       <c r="C63" t="s">
         <v>431</v>
       </c>
+      <c r="D63" t="s">
+        <v>2602</v>
+      </c>
       <c r="E63" t="s">
         <v>150</v>
+      </c>
+      <c r="F63" t="s">
+        <v>2602</v>
       </c>
       <c r="G63" s="1">
         <v>0</v>
@@ -27554,8 +27891,14 @@
       <c r="C64" t="s">
         <v>434</v>
       </c>
+      <c r="D64" t="s">
+        <v>2602</v>
+      </c>
       <c r="E64" t="s">
         <v>150</v>
+      </c>
+      <c r="F64" t="s">
+        <v>2602</v>
       </c>
       <c r="G64" s="1">
         <v>0</v>
@@ -27571,8 +27914,14 @@
       <c r="C65" t="s">
         <v>437</v>
       </c>
+      <c r="D65" t="s">
+        <v>2602</v>
+      </c>
       <c r="E65" t="s">
         <v>150</v>
+      </c>
+      <c r="F65" t="s">
+        <v>2602</v>
       </c>
       <c r="G65" s="1">
         <v>0</v>
@@ -27588,8 +27937,14 @@
       <c r="C66" t="s">
         <v>440</v>
       </c>
+      <c r="D66" t="s">
+        <v>2602</v>
+      </c>
       <c r="E66" t="s">
         <v>150</v>
+      </c>
+      <c r="F66" t="s">
+        <v>2602</v>
       </c>
       <c r="G66" s="1">
         <v>0</v>
@@ -27605,8 +27960,14 @@
       <c r="C67" t="s">
         <v>443</v>
       </c>
+      <c r="D67" t="s">
+        <v>2602</v>
+      </c>
       <c r="E67" t="s">
         <v>241</v>
+      </c>
+      <c r="F67" t="s">
+        <v>2602</v>
       </c>
       <c r="G67" s="1">
         <v>0</v>
@@ -27622,8 +27983,14 @@
       <c r="C68" t="s">
         <v>446</v>
       </c>
+      <c r="D68" t="s">
+        <v>2602</v>
+      </c>
       <c r="E68" t="s">
         <v>31</v>
+      </c>
+      <c r="F68" t="s">
+        <v>2602</v>
       </c>
       <c r="G68" s="1">
         <v>0</v>
@@ -27639,8 +28006,14 @@
       <c r="C69" t="s">
         <v>449</v>
       </c>
+      <c r="D69" t="s">
+        <v>2602</v>
+      </c>
       <c r="E69" t="s">
         <v>17</v>
+      </c>
+      <c r="F69" t="s">
+        <v>2602</v>
       </c>
       <c r="G69" s="1">
         <v>0</v>
@@ -27655,6 +28028,9 @@
       </c>
       <c r="C70" t="s">
         <v>452</v>
+      </c>
+      <c r="D70" t="s">
+        <v>2602</v>
       </c>
       <c r="E70" t="s">
         <v>99</v>
@@ -27679,7 +28055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220FCBEE-5E61-436D-9E3E-A4F93F59585E}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J101" sqref="J101"/>
     </sheetView>
   </sheetViews>
@@ -30068,8 +30444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4304FB-380A-45B3-9A3F-8828CE865E10}">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -30164,6 +30540,9 @@
       <c r="E4" t="s">
         <v>39</v>
       </c>
+      <c r="F4" t="s">
+        <v>2602</v>
+      </c>
       <c r="G4" s="1">
         <v>1533</v>
       </c>
@@ -32093,6 +32472,9 @@
       <c r="E88" t="s">
         <v>31</v>
       </c>
+      <c r="F88" t="s">
+        <v>2602</v>
+      </c>
       <c r="G88" s="1">
         <v>1</v>
       </c>
@@ -32130,8 +32512,14 @@
       <c r="C90" t="s">
         <v>2522</v>
       </c>
+      <c r="D90" t="s">
+        <v>2602</v>
+      </c>
       <c r="E90" t="s">
         <v>31</v>
+      </c>
+      <c r="F90" t="s">
+        <v>2602</v>
       </c>
       <c r="G90" s="1">
         <v>0</v>
@@ -32147,6 +32535,9 @@
       <c r="C91" t="s">
         <v>2525</v>
       </c>
+      <c r="D91" t="s">
+        <v>2602</v>
+      </c>
       <c r="E91" t="s">
         <v>623</v>
       </c>
@@ -32167,6 +32558,9 @@
       <c r="C92" t="s">
         <v>995</v>
       </c>
+      <c r="D92" t="s">
+        <v>2602</v>
+      </c>
       <c r="E92" t="s">
         <v>2545</v>
       </c>
@@ -32187,6 +32581,9 @@
       <c r="C93" t="s">
         <v>2544</v>
       </c>
+      <c r="D93" t="s">
+        <v>2602</v>
+      </c>
       <c r="E93" t="s">
         <v>2545</v>
       </c>
@@ -32207,8 +32604,14 @@
       <c r="C94" t="s">
         <v>998</v>
       </c>
+      <c r="D94" t="s">
+        <v>2602</v>
+      </c>
       <c r="E94" t="s">
         <v>150</v>
+      </c>
+      <c r="F94" t="s">
+        <v>2602</v>
       </c>
       <c r="G94" s="1">
         <v>0</v>
@@ -32224,8 +32627,14 @@
       <c r="C95" t="s">
         <v>1004</v>
       </c>
+      <c r="D95" t="s">
+        <v>2602</v>
+      </c>
       <c r="E95" t="s">
         <v>150</v>
+      </c>
+      <c r="F95" t="s">
+        <v>2602</v>
       </c>
       <c r="G95" s="1">
         <v>0</v>
@@ -32241,8 +32650,14 @@
       <c r="C96" t="s">
         <v>2528</v>
       </c>
+      <c r="D96" t="s">
+        <v>2602</v>
+      </c>
       <c r="E96" t="s">
         <v>17</v>
+      </c>
+      <c r="F96" t="s">
+        <v>2602</v>
       </c>
       <c r="G96" s="1">
         <v>0</v>
@@ -32258,6 +32673,9 @@
       <c r="C97" t="s">
         <v>1013</v>
       </c>
+      <c r="D97" t="s">
+        <v>2602</v>
+      </c>
       <c r="E97" t="s">
         <v>150</v>
       </c>
@@ -32278,6 +32696,9 @@
       <c r="C98" t="s">
         <v>2531</v>
       </c>
+      <c r="D98" t="s">
+        <v>2602</v>
+      </c>
       <c r="E98" t="s">
         <v>99</v>
       </c>
@@ -32298,8 +32719,14 @@
       <c r="C99" t="s">
         <v>1016</v>
       </c>
+      <c r="D99" t="s">
+        <v>2602</v>
+      </c>
       <c r="E99" t="s">
         <v>195</v>
+      </c>
+      <c r="F99" t="s">
+        <v>2602</v>
       </c>
       <c r="G99" s="1">
         <v>0</v>
@@ -32315,6 +32742,9 @@
       <c r="C100" t="s">
         <v>1019</v>
       </c>
+      <c r="D100" t="s">
+        <v>2602</v>
+      </c>
       <c r="E100" t="s">
         <v>195</v>
       </c>
@@ -32335,8 +32765,14 @@
       <c r="C101" t="s">
         <v>1022</v>
       </c>
+      <c r="D101" t="s">
+        <v>2602</v>
+      </c>
       <c r="E101" t="s">
         <v>195</v>
+      </c>
+      <c r="F101" t="s">
+        <v>2602</v>
       </c>
       <c r="G101" s="1">
         <v>0</v>
@@ -32352,6 +32788,9 @@
       <c r="C102" t="s">
         <v>2534</v>
       </c>
+      <c r="D102" t="s">
+        <v>2602</v>
+      </c>
       <c r="E102" t="s">
         <v>56</v>
       </c>
@@ -32372,8 +32811,14 @@
       <c r="C103" t="s">
         <v>1040</v>
       </c>
+      <c r="D103" t="s">
+        <v>2602</v>
+      </c>
       <c r="E103" t="s">
         <v>252</v>
+      </c>
+      <c r="F103" t="s">
+        <v>2602</v>
       </c>
       <c r="G103" s="1">
         <v>0</v>
@@ -32396,8 +32841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3E13CA-8F01-4AB2-8F72-B32DE791032C}">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J92" sqref="J92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -33940,6 +34385,9 @@
       <c r="E67" t="s">
         <v>99</v>
       </c>
+      <c r="F67" t="s">
+        <v>2602</v>
+      </c>
       <c r="G67" s="1">
         <v>9</v>
       </c>
@@ -34351,6 +34799,9 @@
       <c r="E85" t="s">
         <v>56</v>
       </c>
+      <c r="F85" t="s">
+        <v>2602</v>
+      </c>
       <c r="G85" s="1">
         <v>2</v>
       </c>
@@ -34486,6 +34937,9 @@
       <c r="E91" t="s">
         <v>72</v>
       </c>
+      <c r="F91" t="s">
+        <v>2602</v>
+      </c>
       <c r="G91" s="1">
         <v>1</v>
       </c>
@@ -34551,6 +35005,9 @@
       </c>
       <c r="E94" t="s">
         <v>45</v>
+      </c>
+      <c r="F94" t="s">
+        <v>2602</v>
       </c>
       <c r="G94" s="1">
         <v>1</v>

</xml_diff>